<commit_message>
added documents and presentations
</commit_message>
<xml_diff>
--- a/AI Testing 2.xlsx
+++ b/AI Testing 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmcke\Documents\gitStuff\FYP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CDF4BDF-8A2F-42A6-B59D-B682C36C58E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786A7B8D-A337-45F4-B3F6-0CA16E1136B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5830,6 +5830,46 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Testing</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Accuracy</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> of Neural Network</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5905,10 +5945,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$13</c:f>
+              <c:f>Sheet1!$D$3:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -5941,16 +5981,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$J$3:$J$13</c:f>
+              <c:f>Sheet1!$J$3:$J$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>50</c:v>
                 </c:pt>
@@ -5983,6 +6026,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6026,6 +6072,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Number of  Training Trials</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -6071,6 +6172,7 @@
         <c:axId val="233941728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -6088,6 +6190,68 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>% </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Accuracy</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -13269,8 +13433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:M162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F128" sqref="F128"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>